<commit_message>
Improvements in writing the excel but still python does not let it go ;/
</commit_message>
<xml_diff>
--- a/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
+++ b/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
@@ -63,7 +63,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -73,6 +73,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>

<commit_message>
Improved calc_main_part_redundancy, calc_benefit_redundancy and introduced calc_redundancy for less redundant code.
</commit_message>
<xml_diff>
--- a/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
+++ b/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
@@ -7,12 +7,12 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="False Positives Negatives" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="True Positives" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Only US-True Pos." sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'False Positives Negatives'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'True Positives'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -63,7 +63,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -73,9 +73,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">

</xml_diff>

<commit_message>
Repaired Excel Export and Repaied TP, FP, TN, FN calculation
</commit_message>
<xml_diff>
--- a/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
+++ b/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>gpt-3.5-turbo</t>
+          <t>gpt-4-turbo</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -540,14 +540,14 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>326</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>353</v>
+        <v>3</v>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.) The redundancy arises from the repetition of the concept of user verification expressed in slightly different ways for emphasis or to cater to different audiences.
+          <t xml:space="preserve">0.) Dummy Value Describtion
 1.) The redundancy here stems from the repetition of the testing action and the tested entity, expressed in slightly different ways, likely for emphasis or to accommodate different perspectives
 </t>
         </is>
@@ -561,7 +561,7 @@
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> as a staff member, i want to assign an application for detailed review, so that i can #review# them for #compliance# and subsequently approved or denied.</t>
+          <t>No text found in source</t>
         </is>
       </c>
       <c r="J2" s="3" t="inlineStr">
@@ -573,7 +573,66 @@
       </c>
       <c r="K2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> as a plan review staff member, i want to review plans, so that i can #review# them for #compliance# and either approve, or fail or deny the plans and record any conditions, clearances, or corrections needed from the applicant.</t>
+          <t>No text found in source</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>00</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>gpt-4-turbo</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Benefit</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.) The redundancy in these sentences lies in the repetition of the action ('login') and the destination ('webpage' and 'website'), which convey the same idea using slightly different wording.
+1.) Dummy Value Describtion
+</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.) I can login into the webpage.
+1.) I can print a document
+</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>No text found in source</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.) I could login into the website
+1.) I can give the order to print
+</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>No text found in source</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Export to Excerl of the results
</commit_message>
<xml_diff>
--- a/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
+++ b/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
@@ -7,12 +7,14 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Only US-False Pos. Neg." sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Only US-True Pos." sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-Result sheet " sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Only US-False Pos. Neg." sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Only US-True Pos." sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-False Pos. Neg.'!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Only US-Result sheet '!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Only US-False Pos. Neg.'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Only US-True Pos.'!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -439,7 +441,366 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.1" customWidth="1" min="1" max="1"/>
+    <col width="25.5" customWidth="1" min="2" max="2"/>
+    <col width="16.8" customWidth="1" min="3" max="3"/>
+    <col width="13.2" customWidth="1" min="4" max="4"/>
+    <col width="19.2" customWidth="1" min="5" max="5"/>
+    <col width="20.4" customWidth="1" min="6" max="6"/>
+    <col width="20.8" customWidth="1" min="7" max="7"/>
+    <col width="22.1" customWidth="1" min="8" max="8"/>
+    <col width="13.2" customWidth="1" min="9" max="9"/>
+    <col width="9.6" customWidth="1" min="10" max="10"/>
+    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="15.6" customWidth="1" min="13" max="13"/>
+    <col width="15.6" customWidth="1" min="14" max="14"/>
+    <col width="25.2" customWidth="1" min="15" max="15"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Redundancy Part</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Ground Truth</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Predicted</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>True Positives</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>False Positives</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>True Negatives</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>False Negatives</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>F1 Score</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Sensitivity</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Specificity</t>
+        </is>
+      </c>
+      <c r="O1" s="2" t="inlineStr">
+        <is>
+          <t>False Positive Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>ChatGPT 3.5. Turbo</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Main Part</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>[0. 1.]</t>
+        </is>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>[1. 0.]</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>0.</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>ChatGPT 3.5. Turbo</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Benefit</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>[1. 1.]</t>
+        </is>
+      </c>
+      <c r="J3" s="3" t="inlineStr">
+        <is>
+          <t>[1. 0.]</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>ChatGPT 4 Turbo</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Main Part</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>[0. 1.]</t>
+        </is>
+      </c>
+      <c r="J4" s="3" t="inlineStr">
+        <is>
+          <t>[1. 0.]</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>0.</t>
+        </is>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>ChatGPT 4 Turbo</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Benefit</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>[0]</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="inlineStr">
+        <is>
+          <t>[0. 1.]</t>
+        </is>
+      </c>
+      <c r="J5" s="3" t="inlineStr">
+        <is>
+          <t>[1. 0.]</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>0.</t>
+        </is>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -459,8 +820,6 @@
     <col width="96" customWidth="1" min="9" max="9"/>
     <col width="32.4" customWidth="1" min="10" max="10"/>
     <col width="96" customWidth="1" min="11" max="11"/>
-    <col width="84" customWidth="1" min="12" max="12"/>
-    <col width="44.4" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -519,16 +878,6 @@
           <t>Refered Text 2 from formal Approach or Original Text in case of false positive</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Refered Text 1 by ChatGPT or Original Text in case of false positive</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Refered Text 1 from formal Approach</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -564,8 +913,16 @@
 </t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr"/>
-      <c r="I2" s="3" t="inlineStr"/>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="I2" s="3" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
       <c r="J2" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) As an application User, I want to verify that I am who I am
@@ -578,18 +935,6 @@
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
       </c>
-      <c r="L2" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.) As a User, I want to verify myself
-1.) As a software tester, I want to begin user testing
-</t>
-        </is>
-      </c>
-      <c r="M2" s="3" t="inlineStr">
-        <is>
-          <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -625,8 +970,16 @@
 </t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr"/>
-      <c r="I3" s="3" t="inlineStr"/>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="I3" s="3" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
       <c r="J3" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.) I could login into the website
@@ -639,26 +992,14 @@
           <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
         </is>
       </c>
-      <c r="L3" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.) I can login into the webpage.
-1.) I can print a document
-</t>
-        </is>
-      </c>
-      <c r="M3" s="3" t="inlineStr">
-        <is>
-          <t>As a developer, I want to have the subdomain beta.nsf.gov be set up, so that I can deploy a beta site to it.</t>
-        </is>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1"/>
+  <autoFilter ref="A1:K1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Finished Analyse Script for US without annotations
</commit_message>
<xml_diff>
--- a/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
+++ b/redundanciesbyannotations/output_detections_highlighting_without_annotations.xlsx
@@ -65,7 +65,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -74,6 +74,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,18 +453,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9.1" customWidth="1" min="1" max="1"/>
+    <col width="10.5" customWidth="1" min="1" max="1"/>
     <col width="25.5" customWidth="1" min="2" max="2"/>
-    <col width="16.8" customWidth="1" min="3" max="3"/>
+    <col width="21" customWidth="1" min="3" max="3"/>
     <col width="13.2" customWidth="1" min="4" max="4"/>
     <col width="19.2" customWidth="1" min="5" max="5"/>
     <col width="20.4" customWidth="1" min="6" max="6"/>
-    <col width="20.8" customWidth="1" min="7" max="7"/>
-    <col width="22.1" customWidth="1" min="8" max="8"/>
+    <col width="19.2" customWidth="1" min="7" max="7"/>
+    <col width="20.4" customWidth="1" min="8" max="8"/>
     <col width="13.2" customWidth="1" min="9" max="9"/>
     <col width="9.6" customWidth="1" min="10" max="10"/>
     <col width="12" customWidth="1" min="11" max="11"/>
-    <col width="12" customWidth="1" min="12" max="12"/>
+    <col width="15" customWidth="1" min="12" max="12"/>
     <col width="15.6" customWidth="1" min="13" max="13"/>
     <col width="15.6" customWidth="1" min="14" max="14"/>
     <col width="25.2" customWidth="1" min="15" max="15"/>
@@ -817,63 +820,63 @@
     <col width="20.4" customWidth="1" min="6" max="6"/>
     <col width="27.3" customWidth="1" min="7" max="7"/>
     <col width="35.1" customWidth="1" min="8" max="8"/>
-    <col width="96" customWidth="1" min="9" max="9"/>
+    <col width="48" customWidth="1" min="9" max="9"/>
     <col width="32.4" customWidth="1" min="10" max="10"/>
-    <col width="96" customWidth="1" min="11" max="11"/>
+    <col width="48" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Execution Run</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>False Type</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Main Part or Benefit</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>User Story Id 1</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>User Story Id 2</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Reason from ChatGPT</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Refered Text 1 by ChatGPT</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Refered Text 1 from formal Approach or Original Text in case of false positive</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Refered Text 2 by ChatGPT</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>Refered Text 2 from formal Approach or Original Text in case of false positive</t>
         </is>
@@ -915,12 +918,16 @@
       </c>
       <c r="H2" s="3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t xml:space="preserve">0.) As a User, I want to verify myself
+1.) As a software tester, I want to begin user testing
+</t>
         </is>
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t xml:space="preserve">0.) As a User, I want to verify myself
+1.) As a software tester, I want to begin user testing
+</t>
         </is>
       </c>
       <c r="J2" s="3" t="inlineStr">
@@ -972,12 +979,16 @@
       </c>
       <c r="H3" s="3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t xml:space="preserve">0.) I can login into the webpage.
+1.) I can print a document
+</t>
         </is>
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>str</t>
+          <t xml:space="preserve">0.) I can login into the webpage.
+1.) I can print a document
+</t>
         </is>
       </c>
       <c r="J3" s="3" t="inlineStr">
@@ -1019,7 +1030,7 @@
     <col width="26.4" customWidth="1" min="3" max="3"/>
     <col width="20.4" customWidth="1" min="4" max="4"/>
     <col width="20.4" customWidth="1" min="5" max="5"/>
-    <col width="25.2" customWidth="1" min="6" max="6"/>
+    <col width="27.3" customWidth="1" min="6" max="6"/>
     <col width="35.1" customWidth="1" min="7" max="7"/>
     <col width="48.1" customWidth="1" min="8" max="8"/>
     <col width="32.4" customWidth="1" min="9" max="9"/>

</xml_diff>